<commit_message>
added file figures/nasashit 2 ROXX/nasashit 2 ROXX.xlsx
</commit_message>
<xml_diff>
--- a/figures/nasashit 2 ROXX/nasashit 2 ROXX.xlsx
+++ b/figures/nasashit 2 ROXX/nasashit 2 ROXX.xlsx
@@ -57,13 +57,13 @@
     <t>dormitories</t>
   </si>
   <si>
-    <t>3*10*100*1000=3000000</t>
-  </si>
-  <si>
-    <t>125*2*4*5*1000=5000000</t>
-  </si>
-  <si>
-    <t>40*5*10*1000=2000000</t>
+    <t>3*10*100*100=300000</t>
+  </si>
+  <si>
+    <t>125*2*4*5*100=500000</t>
+  </si>
+  <si>
+    <t>40*5*10*100=200000</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>